<commit_message>
Improved the xls generated for taxonomies.
</commit_message>
<xml_diff>
--- a/templates/taxonomy_terms_mapping_template.xlsx
+++ b/templates/taxonomy_terms_mapping_template.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Taxonomy terms mapping" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Comments" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t xml:space="preserve">Source vocabularies (D7)</t>
   </si>
@@ -50,6 +51,9 @@
   </si>
   <si>
     <t xml:space="preserve">Term description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comments</t>
   </si>
 </sst>
 </file>
@@ -59,7 +63,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -104,6 +108,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -131,7 +141,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -167,6 +177,34 @@
       <bottom style="hair"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -193,9 +231,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -211,11 +257,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -248,6 +294,46 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -327,87 +413,408 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3238866396761"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.76113360323887"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="40.8461538461538"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.1902834008097"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="52.753036437247"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.76113360323887"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.76113360323887"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.76113360323887"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="6.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="2" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="6" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7" t="s">
+      <c r="G2" s="8"/>
+      <c r="H2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="9"/>
+      <c r="J2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="K2" s="10"/>
+    </row>
+    <row r="3" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="13" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="16"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="18"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="16"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="18"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="16"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="18"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="16"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="18"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="16"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="18"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="16"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="18"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E11" s="16"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="18"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="16"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="18"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="16"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="18"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E14" s="16"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="18"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="16"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="18"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="16"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="18"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="16"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="18"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E18" s="16"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="18"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="16"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="18"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E20" s="16"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="18"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="16"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="18"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="16"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="18"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="16"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="18"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="16"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="18"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="16"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="18"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="16"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="18"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E27" s="16"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="18"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="16"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="18"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="16"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="18"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="16"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="18"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="16"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="18"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="16"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="18"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="16"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="18"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="16"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="18"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="16"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="18"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="16"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="18"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="20"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -425,4 +832,36 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
D8MT-1100: Update the mapping templates (EWCMS 1.16.0).
</commit_message>
<xml_diff>
--- a/templates/taxonomy_terms_mapping_template.xlsx
+++ b/templates/taxonomy_terms_mapping_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Open vocabulary 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -560,9 +560,9 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="7.92712550607287"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="84.8380566801619"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="85.587044534413"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="9"/>
   </cols>
   <sheetData>
@@ -3765,17 +3765,17 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="45.0971659919028"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="45.5263157894737"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="7.92712550607287"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="95.7651821862348"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="96.6194331983806"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4066,10 +4066,6 @@
   <dataValidations count="6">
     <dataValidation allowBlank="false" error="Please, provide a sting less than or equal to 255 characters for the field &quot;Label&quot;." errorTitle="Invalid data" operator="lessThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2" type="textLength">
       <formula1>255</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C3:C11" type="list">
-      <formula1>"- Select -,Landing page (node.landing_page.ewcms_vocabularies),Call for tenders (node.oe_call_tenders.ewcms_vocabularies),Event (node.oe_event.ewcms_vocabularies),News (node.oe_news.ewcms_vocabularies),Organisation (node.oe_organisation.ewcms_vocabularies),Page (node.oe_page.ewcms_vocabularies),Policy (node.oe_policy.ewcms_vocabularies),Project (node.oe_project.ewcms_vocabularies),Publication (node.oe_publication.ewcms_vocabularies)"</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="C12" type="list">
@@ -4086,6 +4082,10 @@
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="C16" type="list">
       <formula1>"- Select -,TRUE,FALSE"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C3:C11" type="list">
+      <formula1>"- Select -,Landing page (node.landing_page.ewcms_vocabularies),Call for proposals (node.oe_call_proposals.ewcms_vocabularies),Call for tenders (node.oe_call_tenders.ewcms_vocabularies),Event (node.oe_event.ewcms_vocabularies),News (node.oe_news.ewcms_vocabularies),Organisation (node.oe_organisation.ewcms_vocabularies),Page (node.oe_page.ewcms_vocabularies),Policy (node.oe_policy.ewcms_vocabularies),Project (node.oe_project.ewcms_vocabularies),Publication (node.oe_publication.ewcms_vocabularies)"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -4106,17 +4106,17 @@
   </sheetPr>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7813765182186"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="10" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="41.8825910931174"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="54.5222672064777"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="12" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="13" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.74898785425101"/>
@@ -4204,6 +4204,7 @@
       <c r="E4" s="27"/>
       <c r="G4" s="27"/>
       <c r="H4" s="12"/>
+      <c r="I4" s="0"/>
       <c r="J4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4213,6 +4214,7 @@
       <c r="E5" s="27"/>
       <c r="G5" s="27"/>
       <c r="H5" s="28"/>
+      <c r="I5" s="0"/>
       <c r="J5" s="28"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
D8MT-1100: Remove leftover fields.
</commit_message>
<xml_diff>
--- a/templates/taxonomy_terms_mapping_template.xlsx
+++ b/templates/taxonomy_terms_mapping_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Open vocabulary 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
   <si>
     <t xml:space="preserve">Label</t>
   </si>
@@ -159,21 +159,6 @@
   </si>
   <si>
     <t xml:space="preserve">IMPORTANT: An open vocabulary association requires the existence of the referenced open vocabulary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uuid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">langcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weight</t>
   </si>
   <si>
     <t xml:space="preserve">Source vocabularies (D7)</t>
@@ -568,16 +553,16 @@
   </sheetPr>
   <dimension ref="1:21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="1" sqref="C11 A32"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="7.92712550607287"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="86.336032388664"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="87.0890688259109"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="9"/>
   </cols>
   <sheetData>
@@ -3785,19 +3770,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="5" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="45.9554655870445"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="46.3805668016194"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="7.92712550607287"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="97.4777327935223"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="98.336032388664"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="5" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -4069,123 +4054,27 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
       <c r="E20" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
       <c r="E21" s="5" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C43" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -4233,16 +4122,16 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="1" sqref="C11 G15"/>
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.995951417004"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="10" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="42.5263157894737"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="55.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="55.5951417004049"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="12" width="6.74898785425101"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="13" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.74898785425101"/>
@@ -4254,14 +4143,14 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="14" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="15" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
@@ -4276,15 +4165,15 @@
       <c r="D2" s="17"/>
       <c r="E2" s="18"/>
       <c r="F2" s="19" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G2" s="19"/>
       <c r="H2" s="20" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I2" s="20"/>
       <c r="J2" s="21" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="K2" s="21"/>
     </row>
@@ -4293,34 +4182,34 @@
         <v>18</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="J3" s="25" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4669,7 +4558,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
D8MT-1100: Update the taxonomy terms mapping template.
</commit_message>
<xml_diff>
--- a/templates/taxonomy_terms_mapping_template.xlsx
+++ b/templates/taxonomy_terms_mapping_template.xlsx
@@ -5,13 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Open vocabulary 1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Open vocabulary association 1" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Taxonomy terms mapping" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Comments" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Taxonomy terms mapping" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Open vocabulary 1" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Open vocabulary association 1" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +22,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
+  <si>
+    <t xml:space="preserve">Source vocabularies (D7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Destination vocabularies (D8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vocabulary 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vocabulary 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vocabulary …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vocabulary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Term ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Term name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usage (Published entity)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Term description</t>
+  </si>
   <si>
     <t xml:space="preserve">Label</t>
   </si>
@@ -80,9 +109,6 @@
     <t xml:space="preserve">If the selected “Concept Scheme” has subsets that you would like to filter by, please provide a valid one.</t>
   </si>
   <si>
-    <t xml:space="preserve">Vocabulary</t>
-  </si>
-  <si>
     <t xml:space="preserve">target_bundles</t>
   </si>
   <si>
@@ -159,33 +185,6 @@
   </si>
   <si>
     <t xml:space="preserve">IMPORTANT: An open vocabulary association requires the existence of the referenced open vocabulary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source vocabularies (D7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Destination vocabularies (D8)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vocabulary 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vocabulary 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vocabulary …</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Term ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Term name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usage (Published entity)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Term description</t>
   </si>
 </sst>
 </file>
@@ -220,8 +219,16 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FFEEEEEE"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -240,16 +247,8 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FFEEEEEE"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -264,12 +263,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFEEEEEE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF666666"/>
         <bgColor rgb="FF808080"/>
       </patternFill>
@@ -278,6 +271,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB2B2B2"/>
         <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFEEEEEE"/>
       </patternFill>
     </fill>
   </fills>
@@ -362,42 +361,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -414,64 +377,100 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -551,52 +550,488 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:K35"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.74898785425101"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="6.74898785425101"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.74898785425101"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.74898785425101"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="4" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="6.53441295546559"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="10"/>
+      <c r="H2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="12"/>
+    </row>
+    <row r="3" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0"/>
+      <c r="C4" s="0"/>
+      <c r="D4" s="0"/>
+      <c r="E4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="0"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
+      <c r="E5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="0"/>
+      <c r="J5" s="19"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
+      <c r="E6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="19"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0"/>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="19"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0"/>
+      <c r="C8" s="0"/>
+      <c r="D8" s="0"/>
+      <c r="E8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="19"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0"/>
+      <c r="C9" s="0"/>
+      <c r="D9" s="0"/>
+      <c r="E9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="19"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
+      <c r="D10" s="0"/>
+      <c r="E10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="19"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0"/>
+      <c r="C11" s="0"/>
+      <c r="D11" s="0"/>
+      <c r="E11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="19"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+      <c r="D12" s="0"/>
+      <c r="E12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="19"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="19"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+      <c r="D14" s="0"/>
+      <c r="E14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+      <c r="D15" s="0"/>
+      <c r="E15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="19"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0"/>
+      <c r="C16" s="0"/>
+      <c r="D16" s="0"/>
+      <c r="E16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="19"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+      <c r="D17" s="0"/>
+      <c r="E17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="19"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="19"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0"/>
+      <c r="C19" s="0"/>
+      <c r="D19" s="0"/>
+      <c r="E19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="19"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0"/>
+      <c r="C20" s="0"/>
+      <c r="D20" s="0"/>
+      <c r="E20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="19"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0"/>
+      <c r="C21" s="0"/>
+      <c r="D21" s="0"/>
+      <c r="E21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="19"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0"/>
+      <c r="C22" s="0"/>
+      <c r="D22" s="0"/>
+      <c r="E22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="19"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0"/>
+      <c r="C23" s="0"/>
+      <c r="D23" s="0"/>
+      <c r="E23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="19"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0"/>
+      <c r="C24" s="0"/>
+      <c r="D24" s="0"/>
+      <c r="E24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="19"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+      <c r="D25" s="0"/>
+      <c r="E25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="19"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+      <c r="D26" s="0"/>
+      <c r="E26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="19"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0"/>
+      <c r="C27" s="0"/>
+      <c r="D27" s="0"/>
+      <c r="E27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="19"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0"/>
+      <c r="C28" s="0"/>
+      <c r="D28" s="0"/>
+      <c r="E28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="19"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0"/>
+      <c r="C29" s="0"/>
+      <c r="D29" s="0"/>
+      <c r="E29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="19"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0"/>
+      <c r="C30" s="0"/>
+      <c r="D30" s="0"/>
+      <c r="E30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="19"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0"/>
+      <c r="C31" s="0"/>
+      <c r="D31" s="0"/>
+      <c r="E31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="19"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0"/>
+      <c r="C32" s="0"/>
+      <c r="D32" s="0"/>
+      <c r="E32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="19"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0"/>
+      <c r="C33" s="0"/>
+      <c r="D33" s="0"/>
+      <c r="E33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="19"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0"/>
+      <c r="C34" s="0"/>
+      <c r="D34" s="0"/>
+      <c r="E34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="19"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+      <c r="D35" s="0"/>
+      <c r="E35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="1:21"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="7.92712550607287"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="87.0890688259109"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="9"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="20" width="13.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="7.92712550607287"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="20" width="87.8380566801619"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="20" width="9"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
+    <row r="1" s="23" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>5</v>
+      <c r="A2" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>15</v>
       </c>
       <c r="C2" s="0"/>
-      <c r="D2" s="6" t="n">
+      <c r="D2" s="25" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>6</v>
+      <c r="E2" s="24" t="s">
+        <v>16</v>
       </c>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
@@ -1619,19 +2054,19 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
+      <c r="A3" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>18</v>
       </c>
       <c r="C3" s="0"/>
-      <c r="D3" s="6" t="n">
+      <c r="D3" s="25" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>6</v>
+      <c r="E3" s="24" t="s">
+        <v>16</v>
       </c>
       <c r="F3" s="0"/>
       <c r="G3" s="0"/>
@@ -2654,16 +3089,16 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="6" t="n">
+      <c r="A4" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="25" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -3688,57 +4123,57 @@
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" s="7" customFormat="true" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="8" t="n">
+    <row r="5" s="26" customFormat="true" ht="24.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="27" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>14</v>
+      <c r="E5" s="28" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="6" t="n">
+      <c r="A6" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="25" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>17</v>
+      <c r="E6" s="20" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="6" t="n">
+      <c r="A7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="25" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>20</v>
+      <c r="E7" s="20" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="5" t="s">
-        <v>21</v>
+      <c r="E9" s="24" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3765,7 +4200,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3778,303 +4213,303 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="46.3805668016194"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="7.92712550607287"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="98.336032388664"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="5" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="24" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="24" width="11.6761133603239"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="24" width="46.7044534412956"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="7.92712550607287"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="24" width="99.1902834008097"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="24" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
+    <row r="1" s="23" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="6" t="n">
+      <c r="A2" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="25" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>6</v>
+      <c r="E2" s="24" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="6" t="n">
+      <c r="A3" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="25" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>24</v>
+      <c r="E3" s="20" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="6" t="n">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="25" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
+      <c r="E4" s="20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="6" t="n">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="25" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>25</v>
+      <c r="E5" s="20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="6" t="n">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="25" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
+      <c r="E6" s="20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="6" t="n">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="25" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>25</v>
+      <c r="E7" s="20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="6" t="n">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="25" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>25</v>
+      <c r="E8" s="20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="6" t="n">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="25" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>25</v>
+      <c r="E9" s="20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="6" t="n">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="25" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>25</v>
+      <c r="E10" s="20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="6" t="n">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="25" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>25</v>
+      <c r="E11" s="20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="6" t="n">
+      <c r="A12" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="25" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>28</v>
+      <c r="E12" s="20" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="6" t="n">
+      <c r="A13" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="20"/>
+      <c r="D13" s="25" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>30</v>
+      <c r="E13" s="24" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="6" t="n">
+      <c r="A14" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="25" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>33</v>
+      <c r="E14" s="20" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="6" t="n">
+      <c r="A15" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="25" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>37</v>
+      <c r="E15" s="20" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="6" t="n">
+      <c r="A16" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="25" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>39</v>
+      <c r="E16" s="20" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="6" t="n">
+      <c r="A17" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="25" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>42</v>
+      <c r="E17" s="20" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0"/>
       <c r="C18" s="0"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="20"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0"/>
       <c r="C19" s="0"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="20"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0"/>
       <c r="C20" s="0"/>
-      <c r="E20" s="5" t="s">
-        <v>43</v>
+      <c r="E20" s="24" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0"/>
       <c r="C21" s="0"/>
-      <c r="E21" s="5" t="s">
-        <v>44</v>
+      <c r="E21" s="24" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -4112,472 +4547,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:K35"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="42.9554655870445"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="10" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="11" width="55.5951417004049"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="13" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.74898785425101"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="13" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="6.53441295546559"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" s="21"/>
-    </row>
-    <row r="3" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0"/>
-      <c r="C4" s="0"/>
-      <c r="D4" s="0"/>
-      <c r="E4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="0"/>
-      <c r="J4" s="12"/>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0"/>
-      <c r="C5" s="0"/>
-      <c r="D5" s="0"/>
-      <c r="E5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="0"/>
-      <c r="J5" s="28"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0"/>
-      <c r="C6" s="0"/>
-      <c r="D6" s="0"/>
-      <c r="E6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="28"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0"/>
-      <c r="C7" s="0"/>
-      <c r="D7" s="0"/>
-      <c r="E7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="28"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0"/>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="28"/>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0"/>
-      <c r="C9" s="0"/>
-      <c r="D9" s="0"/>
-      <c r="E9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="28"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0"/>
-      <c r="C10" s="0"/>
-      <c r="D10" s="0"/>
-      <c r="E10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="28"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0"/>
-      <c r="C11" s="0"/>
-      <c r="D11" s="0"/>
-      <c r="E11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="28"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0"/>
-      <c r="C12" s="0"/>
-      <c r="D12" s="0"/>
-      <c r="E12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="28"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="D13" s="0"/>
-      <c r="E13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="28"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
-      <c r="D14" s="0"/>
-      <c r="E14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="28"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
-      <c r="C15" s="0"/>
-      <c r="D15" s="0"/>
-      <c r="E15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="28"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0"/>
-      <c r="C16" s="0"/>
-      <c r="D16" s="0"/>
-      <c r="E16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="28"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0"/>
-      <c r="C17" s="0"/>
-      <c r="D17" s="0"/>
-      <c r="E17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="28"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0"/>
-      <c r="C18" s="0"/>
-      <c r="D18" s="0"/>
-      <c r="E18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="28"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0"/>
-      <c r="C19" s="0"/>
-      <c r="D19" s="0"/>
-      <c r="E19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="28"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0"/>
-      <c r="C20" s="0"/>
-      <c r="D20" s="0"/>
-      <c r="E20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="28"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0"/>
-      <c r="C21" s="0"/>
-      <c r="D21" s="0"/>
-      <c r="E21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="28"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0"/>
-      <c r="C22" s="0"/>
-      <c r="D22" s="0"/>
-      <c r="E22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="28"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0"/>
-      <c r="C23" s="0"/>
-      <c r="D23" s="0"/>
-      <c r="E23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="28"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0"/>
-      <c r="C24" s="0"/>
-      <c r="D24" s="0"/>
-      <c r="E24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="28"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0"/>
-      <c r="C25" s="0"/>
-      <c r="D25" s="0"/>
-      <c r="E25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="28"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0"/>
-      <c r="C26" s="0"/>
-      <c r="D26" s="0"/>
-      <c r="E26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="28"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0"/>
-      <c r="C27" s="0"/>
-      <c r="D27" s="0"/>
-      <c r="E27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="28"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0"/>
-      <c r="C28" s="0"/>
-      <c r="D28" s="0"/>
-      <c r="E28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="28"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0"/>
-      <c r="C29" s="0"/>
-      <c r="D29" s="0"/>
-      <c r="E29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="28"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0"/>
-      <c r="C30" s="0"/>
-      <c r="D30" s="0"/>
-      <c r="E30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="28"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0"/>
-      <c r="C31" s="0"/>
-      <c r="D31" s="0"/>
-      <c r="E31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="28"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0"/>
-      <c r="C32" s="0"/>
-      <c r="D32" s="0"/>
-      <c r="E32" s="27"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="27"/>
-      <c r="J32" s="28"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0"/>
-      <c r="C33" s="0"/>
-      <c r="D33" s="0"/>
-      <c r="E33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="28"/>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0"/>
-      <c r="C34" s="0"/>
-      <c r="D34" s="0"/>
-      <c r="E34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="28"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0"/>
-      <c r="C35" s="0"/>
-      <c r="D35" s="0"/>
-      <c r="E35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="28"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>